<commit_message>
Use System.Drawing.Common instead of MetadataExtractor and CoreCompat
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/UsingColors.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/UsingColors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <x:si>
     <x:t>XLColor.Red</x:t>
   </x:si>
@@ -41,9 +41,6 @@
   </x:si>
   <x:si>
     <x:t>XLColor.FromIndex(25)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>XLColor.FromKnownColor(KnownColor.Plum)</x:t>
   </x:si>
   <x:si>
     <x:t>XLColor.FromName("PowderBlue")</x:t>
@@ -71,7 +68,7 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="12">
+  <x:fills count="11">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -106,11 +103,6 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor indexed="25"/>
-      </x:patternFill>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="FFDDA0DD"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
@@ -148,7 +140,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -179,11 +171,8 @@
     <x:xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="10">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -221,10 +210,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -523,7 +508,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B20"/>
+  <x:dimension ref="A1:B18"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -599,16 +584,10 @@
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:2">
-      <x:c r="A19" s="9" t="s"/>
-      <x:c r="B19" s="0" t="s">
+    <x:row r="18" spans="1:2">
+      <x:c r="A18" s="9" t="s"/>
+      <x:c r="B18" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:2">
-      <x:c r="A20" s="10" t="s"/>
-      <x:c r="B20" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>